<commit_message>
2017 07 28 update
</commit_message>
<xml_diff>
--- a/Planning/Specials Layout.xlsx
+++ b/Planning/Specials Layout.xlsx
@@ -13,10 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
-    <sheet name="Symbols" sheetId="5" r:id="rId2"/>
-    <sheet name="Examples" sheetId="4" r:id="rId3"/>
-    <sheet name="Time" sheetId="2" r:id="rId4"/>
-    <sheet name="Food or Drink" sheetId="3" r:id="rId5"/>
+    <sheet name="Food or Drink" sheetId="3" r:id="rId2"/>
+    <sheet name="Time" sheetId="2" r:id="rId3"/>
+    <sheet name="Cuisine" sheetId="6" r:id="rId4"/>
+    <sheet name="Sort By" sheetId="8" r:id="rId5"/>
+    <sheet name="Start" sheetId="7" r:id="rId6"/>
+    <sheet name="Symbols" sheetId="5" r:id="rId7"/>
+    <sheet name="Examples" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Home Screen</t>
-  </si>
-  <si>
-    <t>Home</t>
   </si>
   <si>
     <t>Symbols</t>
@@ -41,32 +41,33 @@
   <si>
     <t>Standard Layout</t>
   </si>
+  <si>
+    <t>Search kicks off the overall search for Specials</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Sort By:</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Most Popular</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="18"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,16 +90,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6347,8 +6345,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="3136445" y="8489128"/>
-            <a:ext cx="2165803" cy="381001"/>
+            <a:off x="2298463" y="8489128"/>
+            <a:ext cx="3003785" cy="381001"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -6388,7 +6386,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mj-lt"/>
               </a:rPr>
-              <a:t>Map</a:t>
+              <a:t>Current       Map Area</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -7377,6 +7375,2367 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342408</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>142007</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="1771650"/>
+          <a:ext cx="3933333" cy="6942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="1819275"/>
+          <a:ext cx="3857625" cy="6848475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>544838</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>72770</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="4812038" cy="644270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="8A3B1F"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>49328</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>83003</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>227920</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>163599</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="658928" y="464003"/>
+          <a:ext cx="3226592" cy="461596"/>
+          <a:chOff x="642939" y="2202656"/>
+          <a:chExt cx="2309812" cy="461596"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rounded Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="642939" y="2202656"/>
+            <a:ext cx="2309812" cy="461596"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="672210" y="2226469"/>
+            <a:ext cx="1475606" cy="376859"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Food</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> or Drink</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>:</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rounded Rectangle 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2182812" y="2202657"/>
+            <a:ext cx="722313" cy="422413"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Both</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>445634</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>96610</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>450701</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>138023</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rounded Rectangle 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4103234" y="477610"/>
+          <a:ext cx="1224267" cy="422413"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Search</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rounded Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="2343150"/>
+          <a:ext cx="3848100" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rounded Rectangle 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="2638424"/>
+          <a:ext cx="3600450" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Food &amp; Drink</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Specials</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rounded Rectangle 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="3200399"/>
+          <a:ext cx="3600450" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Food Specials Only</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rounded Rectangle 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="3762375"/>
+          <a:ext cx="3600450" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Drink</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Specials Only</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>509588</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>423863</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2338388" y="4381500"/>
+          <a:ext cx="523875" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="4000">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1733550" y="1200150"/>
+          <a:ext cx="2571749" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>Select Time</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>551958</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>8657</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885825" y="790575"/>
+          <a:ext cx="3933333" cy="6942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="895350" y="819150"/>
+          <a:ext cx="3857625" cy="6848475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>477976</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>107157</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1087576" y="1733550"/>
+          <a:ext cx="3493950" cy="3050382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561733</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142813</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066800" y="600075"/>
+          <a:ext cx="1933333" cy="495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1009649" y="3200400"/>
+          <a:ext cx="3476625" cy="6000750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="24" name="Group 23"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1076325" y="3448050"/>
+          <a:ext cx="3343275" cy="504825"/>
+          <a:chOff x="1076325" y="3448050"/>
+          <a:chExt cx="3343275" cy="504825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="Rounded Rectangle 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1076325" y="3448050"/>
+            <a:ext cx="3343275" cy="504825"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>American</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="Oval 19"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3835146" y="3524251"/>
+            <a:ext cx="347472" cy="347472"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="8A3B1F"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="30" name="Group 29"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1076325" y="4048125"/>
+          <a:ext cx="3343275" cy="504825"/>
+          <a:chOff x="1076325" y="3448050"/>
+          <a:chExt cx="3343275" cy="504825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="Rounded Rectangle 30"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1076325" y="3448050"/>
+            <a:ext cx="3343275" cy="504825"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Chinese</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="33" name="Oval 32"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3835146" y="3524251"/>
+            <a:ext cx="347472" cy="347472"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="8A3B1F"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="35" name="Group 34"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1076325" y="4648200"/>
+          <a:ext cx="3343275" cy="504825"/>
+          <a:chOff x="1076325" y="3448050"/>
+          <a:chExt cx="3343275" cy="504825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="Rounded Rectangle 35"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1076325" y="3448050"/>
+            <a:ext cx="3343275" cy="504825"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Thai</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="38" name="Oval 37"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3835146" y="3524251"/>
+            <a:ext cx="347472" cy="347472"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="8A3B1F"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="45" name="Group 44"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1076325" y="5248275"/>
+          <a:ext cx="3343275" cy="504825"/>
+          <a:chOff x="1076325" y="3448050"/>
+          <a:chExt cx="3343275" cy="504825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="46" name="Rounded Rectangle 45"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1076325" y="3448050"/>
+            <a:ext cx="3343275" cy="504825"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Pizza</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="48" name="Oval 47"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3835146" y="3524251"/>
+            <a:ext cx="347472" cy="347472"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="8A3B1F"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="50" name="Group 49"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1076325" y="5848350"/>
+          <a:ext cx="3343275" cy="504825"/>
+          <a:chOff x="1076325" y="3448050"/>
+          <a:chExt cx="3343275" cy="504825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="51" name="Rounded Rectangle 50"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1076325" y="3448050"/>
+            <a:ext cx="3343275" cy="504825"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Mexican</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="53" name="Oval 52"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3835146" y="3524251"/>
+            <a:ext cx="347472" cy="347472"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="8A3B1F"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="55" name="Group 54"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1076325" y="6448425"/>
+          <a:ext cx="3343275" cy="504825"/>
+          <a:chOff x="1076325" y="3448050"/>
+          <a:chExt cx="3343275" cy="504825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="56" name="Rounded Rectangle 55"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1076325" y="3448050"/>
+            <a:ext cx="3343275" cy="504825"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Vegetarian</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="58" name="Oval 57"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3835146" y="3524251"/>
+            <a:ext cx="347472" cy="347472"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="8A3B1F"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="60" name="Group 59"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1076325" y="7048500"/>
+          <a:ext cx="3343275" cy="504825"/>
+          <a:chOff x="1076325" y="3448050"/>
+          <a:chExt cx="3343275" cy="504825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="61" name="Rounded Rectangle 60"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1076325" y="3448050"/>
+            <a:ext cx="3343275" cy="504825"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Vietnamese</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="63" name="Oval 62"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3835146" y="3524251"/>
+            <a:ext cx="347472" cy="347472"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="8A3B1F"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="70" name="Group 69"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1076325" y="7648575"/>
+          <a:ext cx="3343275" cy="504825"/>
+          <a:chOff x="1076325" y="3448050"/>
+          <a:chExt cx="3343275" cy="504825"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="71" name="Rounded Rectangle 70"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1076325" y="3448050"/>
+            <a:ext cx="3343275" cy="504825"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Sushi</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="72" name="Group 71"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="3835146" y="3524251"/>
+            <a:ext cx="347472" cy="347472"/>
+            <a:chOff x="8349996" y="4476751"/>
+            <a:chExt cx="347472" cy="347472"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="73" name="Oval 72"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8349996" y="4476751"/>
+              <a:ext cx="347472" cy="347472"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="8A3B1F"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="74" name="Oval 73"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8409432" y="4536187"/>
+              <a:ext cx="228600" cy="228600"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="8A3B1F"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="Down Arrow 80"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2590800" y="8391525"/>
+          <a:ext cx="485775" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="8A3B1F"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>475758</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>18182</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="695325"/>
+          <a:ext cx="3933333" cy="6942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="828675" y="752475"/>
+          <a:ext cx="3857625" cy="6848475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -9513,7 +11872,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -10334,112 +12693,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>608990</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>66143</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="762000"/>
-          <a:ext cx="4876190" cy="4257143"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1733550" y="1200150"/>
-          <a:ext cx="2571749" cy="438150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1"/>
-            <a:t>Select Time</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10706,7 +12959,7 @@
   <dimension ref="B1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10724,6 +12977,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="K4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -10734,12 +13095,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -10749,7 +13110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -10762,41 +13123,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="Home!A1" display="Home"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>